<commit_message>
Updated running time to 16 weeks. Changed time to process one event to 136ms. Changed time to simulated one event to 215 ms. These numbers are what were shown at the 2017 S&T review by Graham.
</commit_message>
<xml_diff>
--- a/computing_model_2017-05.xlsx
+++ b/computing_model_2017-05.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="1160" windowWidth="25600" windowHeight="16060" tabRatio="991"/>
+    <workbookView xWindow="10020" yWindow="0" windowWidth="25660" windowHeight="19380" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="Pass1CPUs">model!$B$10</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,9 +58,6 @@
     <t>weeks</t>
   </si>
   <si>
-    <t>amount of running in a year, fy17: 35+67 days, fy18: 42+10+21 days (see Eugene’s talk, Oct. ‘16 Collab. Mtg.)</t>
-  </si>
-  <si>
     <t>running efficiency</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>MC CPU time per event, generation</t>
   </si>
   <si>
-    <t>per David's email of 11/1, point 2, fy 18 a factor of two more due to G3 → G4 switch</t>
-  </si>
-  <si>
     <t>MC CPU time per event, reconstruction</t>
   </si>
   <si>
@@ -484,9 +478,6 @@
     <t>total data to tape (PB)</t>
   </si>
   <si>
-    <t>Oct. 2016 David benchmark 2016-Broadwell real cores for FY17 and FY18. Benchmark for Spring 2017 data for FY18 and FY19</t>
-  </si>
-  <si>
     <t>fy17(old)</t>
   </si>
   <si>
@@ -494,6 +485,20 @@
   </si>
   <si>
     <t>fy19(new)</t>
+  </si>
+  <si>
+    <t>per David's email of 11/1, point 2, fy 18 a factor of two more due to G3 → G4 switch
+0.215 comes from measurement done in late June/early July 2017 (see e-mail exchange
+between David,Graham, and Richard during this time)</t>
+  </si>
+  <si>
+    <t>Oct. 2016 David benchmark 2016-Broadwell real cores for FY17 and FY18. Benchmark for Spring 2017 data for FY18 and FY19
+The 0.137 comes from benchmarks done by David. The number is actually what Graham used for 2017 S &amp; T review. This corresponds
+to 300Hz on a 36core+36HT computer where the HT are counted as 14% of a core.</t>
+  </si>
+  <si>
+    <t>amount of running in a year, fy17: 35+67 days, fy18: 42+10+21 days (see Eugene’s talk, Oct. ‘16 Collab. Mtg.)
+FY19 has 16 weeks coming from Graham's number used in the 2017 S&amp;T review</t>
   </si>
 </sst>
 </file>
@@ -568,7 +573,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -595,6 +600,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1000,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1027,13 +1042,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -1076,19 +1091,18 @@
         <v>10.428571428571429</v>
       </c>
       <c r="D5" s="4">
-        <f>(42+10+21)/7</f>
-        <v>10.428571428571429</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:7 1025:1025" ht="12" customHeight="1">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3">
         <v>0.5</v>
@@ -1100,12 +1114,12 @@
         <v>0.5</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7 1025:1025" ht="12.25" customHeight="1">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <f>B4*B5/(365.25/7)*B6</f>
@@ -1117,18 +1131,18 @@
       </c>
       <c r="D7">
         <f>D4*D5/(365.25/7)*D6</f>
-        <v>8993.8398357289534</v>
+        <v>13798.76796714579</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7 1025:1025" ht="12.25" customHeight="1">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="5">
         <f>B7*365*24*60*60</f>
@@ -1140,18 +1154,18 @@
       </c>
       <c r="D8" s="5">
         <f>D7*365*24*60*60</f>
-        <v>283629733059.54828</v>
+        <v>435157946611.90967</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7 1025:1025" ht="12.25" customHeight="1">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3">
         <f>1/9.8</f>
@@ -1162,19 +1176,19 @@
         <v>0.1020408163265306</v>
       </c>
       <c r="D9" s="3">
-        <f>1/5.6</f>
-        <v>0.17857142857142858</v>
+        <f>(36*1.14)/300</f>
+        <v>0.1368</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:7 1025:1025" ht="12.25" customHeight="1">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <f>B7*B9</f>
@@ -1186,18 +1200,18 @@
       </c>
       <c r="D10">
         <f>D7*D9</f>
-        <v>1606.0428278087418</v>
+        <v>1887.6714579055442</v>
       </c>
       <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7 1025:1025" ht="12.25" customHeight="1">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3">
         <f>(11.5+2.3*2)*1000</f>
@@ -1211,15 +1225,15 @@
         <v>16800</v>
       </c>
       <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7 1025:1025" ht="12.25" customHeight="1">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <f>B4*B11/1000000</f>
@@ -1234,15 +1248,15 @@
         <v>1512</v>
       </c>
       <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7 1025:1025" ht="12.25" customHeight="1">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="6">
         <f>B8*B11</f>
@@ -1254,18 +1268,18 @@
       </c>
       <c r="D13" s="6">
         <f>D8*D11</f>
-        <v>4764979515400411</v>
+        <v>7310653503080082</v>
       </c>
       <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7 1025:1025">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <f>B13/1000000000000</f>
@@ -1277,18 +1291,18 @@
       </c>
       <c r="D14">
         <f>D13/1000000000000</f>
-        <v>4764.9795154004114</v>
+        <v>7310.6535030800824</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7 1025:1025">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="3">
         <v>0.05</v>
@@ -1300,12 +1314,12 @@
         <v>0.05</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7 1025:1025">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
@@ -1317,12 +1331,12 @@
         <v>2</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -1334,12 +1348,12 @@
         <v>2</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <f>B15*B17*B10</f>
@@ -1351,18 +1365,18 @@
       </c>
       <c r="D18">
         <f>D15*D17*D10</f>
-        <v>160.6042827808742</v>
+        <v>188.76714579055442</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19">
         <f>B16*B10</f>
@@ -1374,19 +1388,19 @@
       </c>
       <c r="D19">
         <f>D16*D10</f>
-        <v>3212.0856556174836</v>
+        <v>3775.3429158110885</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3">
         <v>0.1</v>
@@ -1398,12 +1412,12 @@
         <v>0.1</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="3">
         <v>0.1</v>
@@ -1415,12 +1429,12 @@
         <v>0.1</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="3">
         <v>5</v>
@@ -1432,12 +1446,12 @@
         <v>5</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <f>B20*B10</f>
@@ -1449,18 +1463,18 @@
       </c>
       <c r="D23">
         <f>D20*D10</f>
-        <v>160.6042827808742</v>
+        <v>188.76714579055442</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3">
         <v>2</v>
@@ -1472,12 +1486,12 @@
         <v>2</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25">
         <f>B22*B23*B24</f>
@@ -1489,18 +1503,18 @@
       </c>
       <c r="D25">
         <f>D22*D23*D24</f>
-        <v>1606.042827808742</v>
+        <v>1887.6714579055442</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <f>B50*B21</f>
@@ -1512,15 +1526,15 @@
       </c>
       <c r="D26">
         <f>D50*D21</f>
-        <v>3.0219301848049285</v>
+        <v>4.6363860369609853</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27">
         <f>B26*B22*B24*$G2/1000000000</f>
@@ -1532,35 +1546,35 @@
       </c>
       <c r="D27">
         <f>D26*D22*D24*$G2/1000000000</f>
-        <v>0.95364864000000016</v>
+        <v>1.46313216</v>
       </c>
       <c r="E27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="14" customFormat="1" ht="36">
+      <c r="A28" s="14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="3">
+      <c r="B28" s="15">
         <f>1/18</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="15">
         <f>2*(1/18)</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="D28" s="3">
-        <f>2*(1/18)</f>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>59</v>
+      <c r="D28" s="15">
+        <f>0.215</f>
+        <v>0.215</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29">
         <f>B9</f>
@@ -1572,12 +1586,12 @@
       </c>
       <c r="D29">
         <f>D9</f>
-        <v>0.17857142857142858</v>
+        <v>0.1368</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30">
         <f>B28/B9</f>
@@ -1589,18 +1603,18 @@
       </c>
       <c r="D30">
         <f>D28/D9</f>
-        <v>0.62222222222222212</v>
+        <v>1.5716374269005846</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31">
         <f>B29/B9</f>
@@ -1615,12 +1629,12 @@
         <v>1</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" s="3">
         <v>2</v>
@@ -1632,12 +1646,12 @@
         <v>2</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:6 1025:1025">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B33">
         <v>18000</v>
@@ -1649,15 +1663,15 @@
         <v>18000</v>
       </c>
       <c r="E33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:6 1025:1025">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B34" s="3">
         <v>2</v>
@@ -1669,12 +1683,12 @@
         <v>2</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:6 1025:1025">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35">
         <f>B7*B32*B34</f>
@@ -1686,18 +1700,18 @@
       </c>
       <c r="D35">
         <f>D7*D32*D34</f>
-        <v>35975.359342915814</v>
+        <v>55195.07186858316</v>
       </c>
       <c r="E35" t="s">
         <v>7</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:6 1025:1025">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B36">
         <f>B32*B10*(B30+B31)*B34</f>
@@ -1709,18 +1723,18 @@
       </c>
       <c r="D36">
         <f>D32*D10*(D30+D31)*D34</f>
-        <v>10421.433460447835</v>
+        <v>19417.626283367557</v>
       </c>
       <c r="E36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:6 1025:1025">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B37">
         <f>B33*B48</f>
@@ -1735,15 +1749,15 @@
         <v>3600</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:6 1025:1025">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B38">
         <f>B35*B37/1000000</f>
@@ -1755,15 +1769,15 @@
       </c>
       <c r="D38">
         <f>D35*D37/1000000</f>
-        <v>129.51129363449692</v>
+        <v>198.70225872689937</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:6 1025:1025">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39">
         <f>B38*$G2/1000000000</f>
@@ -1775,15 +1789,15 @@
       </c>
       <c r="D39">
         <f>D38*$G2/1000000000</f>
-        <v>4.0870655999999999</v>
+        <v>6.2705663999999999</v>
       </c>
       <c r="E39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:6 1025:1025">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B40" s="3">
         <v>0.1</v>
@@ -1795,12 +1809,12 @@
         <v>0.1</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:6 1025:1025">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B41" s="3">
         <v>10</v>
@@ -1812,12 +1826,12 @@
         <v>10</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:6 1025:1025">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B42">
         <f>B40*B10*B41</f>
@@ -1829,18 +1843,18 @@
       </c>
       <c r="D42">
         <f>D40*D10*D41</f>
-        <v>1606.042827808742</v>
+        <v>1887.6714579055442</v>
       </c>
       <c r="E42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:6 1025:1025" s="8" customFormat="1">
       <c r="A43" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" s="9">
         <f>B18+B19+B25+B36+B42</f>
@@ -1852,19 +1866,19 @@
       </c>
       <c r="D43" s="9">
         <f>D18+D19+D25+D36+D42</f>
-        <v>17006.209054463678</v>
+        <v>27157.07926078029</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AMK43"/>
     </row>
     <row r="44" spans="1:6 1025:1025">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B44">
         <f>B43-B36</f>
@@ -1876,18 +1890,18 @@
       </c>
       <c r="D44">
         <f>D43-D36</f>
-        <v>6584.7755940158422</v>
+        <v>7739.4529774127332</v>
       </c>
       <c r="E44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:6 1025:1025">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" s="3">
         <v>100</v>
@@ -1899,15 +1913,15 @@
         <v>100</v>
       </c>
       <c r="E45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:6 1025:1025">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B46" s="3">
         <v>3</v>
@@ -1919,15 +1933,15 @@
         <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:6 1025:1025">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47">
         <f>B7*B11/B45/1000000</f>
@@ -1939,12 +1953,12 @@
       </c>
       <c r="D47">
         <f>D7*D11/D45/1000000</f>
-        <v>1.5109650924024642</v>
+        <v>2.3181930184804926</v>
       </c>
     </row>
     <row r="48" spans="1:6 1025:1025">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B48" s="3">
         <v>0.2</v>
@@ -1956,12 +1970,12 @@
         <v>0.2</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B49">
         <f>B48*B11</f>
@@ -1976,15 +1990,15 @@
         <v>3360</v>
       </c>
       <c r="E49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B50">
         <f>B7*B49/1000000</f>
@@ -1996,18 +2010,18 @@
       </c>
       <c r="D50">
         <f>D7*D49/1000000</f>
-        <v>30.219301848049284</v>
+        <v>46.363860369609853</v>
       </c>
       <c r="E50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B51">
         <f>B16*B50*365.25*24*60*60/1000000000</f>
@@ -2019,18 +2033,18 @@
       </c>
       <c r="D51">
         <f>D16*D50*365.25*24*60*60/1000000000</f>
-        <v>1.9072972800000003</v>
+        <v>2.92626432</v>
       </c>
       <c r="E51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B52">
         <f>B15*B7*B49/1000000</f>
@@ -2042,18 +2056,18 @@
       </c>
       <c r="D52">
         <f>D15*D7*D49/1000000</f>
-        <v>1.5109650924024642</v>
+        <v>2.3181930184804926</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B53">
         <f>B17*B52*365.25*24*60*60/1000000000</f>
@@ -2065,18 +2079,18 @@
       </c>
       <c r="D53">
         <f>D17*D52*365.25*24*60*60/1000000000</f>
-        <v>9.5364864000000035E-2</v>
+        <v>0.14631321599999997</v>
       </c>
       <c r="E53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B54">
         <f>B7*(B49+B11)/(B45*1000000)</f>
@@ -2088,18 +2102,18 @@
       </c>
       <c r="D54">
         <f>D7*(D49+D11)/(D45*1000000)</f>
-        <v>1.8131581108829571</v>
+        <v>2.7818316221765911</v>
       </c>
       <c r="E54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55">
         <f>B16*B54</f>
@@ -2111,18 +2125,18 @@
       </c>
       <c r="D55">
         <f>D16*D54</f>
-        <v>3.6263162217659142</v>
+        <v>5.5636632443531822</v>
       </c>
       <c r="E55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B56">
         <f>B15*B54</f>
@@ -2134,18 +2148,18 @@
       </c>
       <c r="D56">
         <f>D15*D54</f>
-        <v>9.0657905544147863E-2</v>
+        <v>0.13909158110882955</v>
       </c>
       <c r="E56" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B57">
         <f>B17*B56</f>
@@ -2157,18 +2171,18 @@
       </c>
       <c r="D57">
         <f>D17*D56</f>
-        <v>0.18131581108829573</v>
+        <v>0.2781831622176591</v>
       </c>
       <c r="E57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B58">
         <f>B7*B49/(10*1000000)</f>
@@ -2180,18 +2194,18 @@
       </c>
       <c r="D58">
         <f>D7*D49/(10*1000000)</f>
-        <v>3.0219301848049285</v>
+        <v>4.6363860369609853</v>
       </c>
       <c r="E58" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59">
         <f>B22*B58*B20</f>
@@ -2203,18 +2217,18 @@
       </c>
       <c r="D59">
         <f>D22*D58*D20</f>
-        <v>1.5109650924024642</v>
+        <v>2.3181930184804926</v>
       </c>
       <c r="E59" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B60">
         <f>(B58+B59)*B24</f>
@@ -2226,18 +2240,18 @@
       </c>
       <c r="D60">
         <f>(D58+D59)*D24</f>
-        <v>9.0657905544147859</v>
+        <v>13.909158110882956</v>
       </c>
       <c r="E60" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B61">
         <f>B38/B45</f>
@@ -2249,18 +2263,18 @@
       </c>
       <c r="D61">
         <f>D38/D45</f>
-        <v>1.2951129363449692</v>
+        <v>1.9870225872689937</v>
       </c>
       <c r="E61" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B62">
         <f>B47+B55+B57+B60+B61</f>
@@ -2272,15 +2286,15 @@
       </c>
       <c r="D62">
         <f>D47+D55+D57+D60+D61</f>
-        <v>15.679500616016428</v>
+        <v>24.056220123203282</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B63" s="3">
         <v>20</v>
@@ -2292,15 +2306,15 @@
         <v>20</v>
       </c>
       <c r="E63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B64">
         <f>B63*B41</f>
@@ -2315,15 +2329,15 @@
         <v>200</v>
       </c>
       <c r="E64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B65">
         <f>B14/1000+B51+B53+B27+B39</f>
@@ -2335,7 +2349,7 @@
       </c>
       <c r="D65">
         <f>D14/1000+D51+D53+D27+D39</f>
-        <v>11.808355899400413</v>
+        <v>18.11692959908008</v>
       </c>
     </row>
   </sheetData>
@@ -2373,7 +2387,7 @@
     </row>
     <row r="2" spans="1:5" ht="12.25" customHeight="1">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" s="3">
         <f>model!B5</f>
@@ -2386,7 +2400,7 @@
     </row>
     <row r="3" spans="1:5" ht="12.25" customHeight="1">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3">
         <f>7*B2</f>
@@ -2397,7 +2411,7 @@
         <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E3" s="3">
         <v>2</v>
@@ -2405,7 +2419,7 @@
     </row>
     <row r="4" spans="1:5" ht="12.25" customHeight="1">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <f>model!B6</f>
@@ -2416,7 +2430,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E4">
         <f>24*60*60</f>
@@ -2425,7 +2439,7 @@
     </row>
     <row r="5" spans="1:5" ht="12.25" customHeight="1">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5" s="5">
         <f>B3*B4*$E$4</f>
@@ -2436,7 +2450,7 @@
         <v>3153600</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E5">
         <v>365.25</v>
@@ -2444,7 +2458,7 @@
     </row>
     <row r="6" spans="1:5" ht="12.25" customHeight="1">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>20000</v>
@@ -2453,7 +2467,7 @@
         <v>20000</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E6">
         <v>10000</v>
@@ -2461,7 +2475,7 @@
     </row>
     <row r="7" spans="1:5" ht="12.25" customHeight="1">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B7" s="5">
         <f>B5*B6</f>
@@ -2472,7 +2486,7 @@
         <v>63072000000</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -2482,7 +2496,7 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E8">
         <v>18000</v>
@@ -2490,7 +2504,7 @@
     </row>
     <row r="9" spans="1:5" ht="12.25" customHeight="1">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B9">
         <f>model!B9</f>
@@ -2501,7 +2515,7 @@
         <v>0.1020408163265306</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E9">
         <v>0.2</v>
@@ -2509,7 +2523,7 @@
     </row>
     <row r="10" spans="1:5" ht="12.25" customHeight="1">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10">
         <f>B7*B9/$E$4/$E$5</f>
@@ -2522,7 +2536,7 @@
     </row>
     <row r="11" spans="1:5" ht="12.25" customHeight="1">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B11">
         <f>B7*B9/$E$4/$E$6</f>
@@ -2535,7 +2549,7 @@
     </row>
     <row r="13" spans="1:5" ht="12.25" customHeight="1">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13">
         <f>model!B28</f>
@@ -2548,7 +2562,7 @@
     </row>
     <row r="14" spans="1:5" ht="12.25" customHeight="1">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B14">
         <f>B9</f>
@@ -2561,7 +2575,7 @@
     </row>
     <row r="15" spans="1:5" ht="12.25" customHeight="1">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B15">
         <f>B7*$E$7*(B14+B13)/$E$4/$E$6</f>
@@ -2574,7 +2588,7 @@
     </row>
     <row r="17" spans="1:3" ht="12.25" customHeight="1">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B17">
         <f>B11+B15</f>
@@ -2587,7 +2601,7 @@
     </row>
     <row r="23" spans="1:3" ht="12.25" customHeight="1">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B23">
         <f>B7*$E8</f>
@@ -2600,7 +2614,7 @@
     </row>
     <row r="24" spans="1:3" ht="12.25" customHeight="1">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B24">
         <f>B23/1000000000000000</f>
@@ -2613,7 +2627,7 @@
     </row>
     <row r="25" spans="1:3" ht="12.25" customHeight="1">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B25">
         <f>B24*$E9</f>
@@ -2626,7 +2640,7 @@
     </row>
     <row r="26" spans="1:3" ht="12.25" customHeight="1">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26">
         <f>B24*(1+0.2*(2*1+2*2+2*0.05+5*0.1))</f>

</xml_diff>